<commit_message>
Laborator 12.10.2022 - Bazele WFA - un program cu niste controale de baza, si folosirea unui Bitmap si Graphics; crearea primului joc cu ce am invatat - X si O
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718AD014-5F4F-4024-8E52-83943BCCAF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B116AEF2-A77E-4C17-920C-FBCBAF88AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Toda Camelia</t>
   </si>
   <si>
-    <t>Let Raul Ivan</t>
-  </si>
-  <si>
     <t>Ifrim Alexandru</t>
   </si>
   <si>
@@ -129,6 +126,18 @@
   </si>
   <si>
     <t>sapt 14</t>
+  </si>
+  <si>
+    <t>Rat Adrian</t>
+  </si>
+  <si>
+    <t>Bordas Norbert</t>
+  </si>
+  <si>
+    <t>Ivan Let Raul</t>
+  </si>
+  <si>
+    <t>Mailot Dorian</t>
   </si>
 </sst>
 </file>
@@ -172,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -195,16 +204,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,51 +558,51 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -592,6 +615,9 @@
       <c r="B3" t="b">
         <v>1</v>
       </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -622,12 +648,18 @@
       <c r="B6" t="b">
         <v>1</v>
       </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -671,6 +703,9 @@
       <c r="B11" t="b">
         <v>1</v>
       </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -725,6 +760,30 @@
         <v>15</v>
       </c>
       <c r="C18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 18.10 - Colectii
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357E6F86-AEFC-4499-B662-65C8FB650519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6254886-E9F8-486E-958E-018BD510ECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -545,7 +545,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,6 +632,9 @@
       <c r="C4" t="b">
         <v>1</v>
       </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -676,6 +679,9 @@
       <c r="C8" t="b">
         <v>1</v>
       </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -687,6 +693,9 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -709,6 +718,9 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -741,6 +753,9 @@
       <c r="C15" t="b">
         <v>1</v>
       </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -750,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -758,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -766,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -774,19 +789,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 19.10 - Am inceput implementarea unui shooter. Apar niste inamici pe care ii putem impusca si invinge, iar cand toti sunt invinsi, castigam.
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6254886-E9F8-486E-958E-018BD510ECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6AD204-30FC-4B47-80CC-65F90E9BB070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>Mailot Dorian</t>
+  </si>
+  <si>
+    <t>Buda Raul</t>
+  </si>
+  <si>
+    <t>Lazea Denisa</t>
+  </si>
+  <si>
+    <t>Costea Raul</t>
+  </si>
+  <si>
+    <t>Petrut Andreea</t>
   </si>
 </sst>
 </file>
@@ -181,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -217,17 +229,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,6 +634,9 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -621,6 +648,9 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -657,6 +687,9 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -668,6 +701,9 @@
       <c r="C7" t="b">
         <v>1</v>
       </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -707,6 +743,9 @@
       <c r="C10" t="b">
         <v>1</v>
       </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -729,6 +768,9 @@
       <c r="C12" t="b">
         <v>1</v>
       </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -772,6 +814,9 @@
       <c r="C17" t="b">
         <v>1</v>
       </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -788,6 +833,9 @@
       <c r="C19" t="b">
         <v>1</v>
       </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -808,6 +856,38 @@
         <v>1</v>
       </c>
       <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 25.10.2022 - folositul metodelor in primul program realizat pana acum
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6AD204-30FC-4B47-80CC-65F90E9BB070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4ADF78-6BD9-40FC-97D8-D8A65E82B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Petrut Andreea</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lucaciu Vlad</t>
+  </si>
+  <si>
+    <t>Marta George</t>
   </si>
 </sst>
 </file>
@@ -173,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +201,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -220,9 +235,45 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -236,28 +287,117 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -566,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,321 +717,792 @@
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="P1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="16">
+        <f>B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="16">
+        <f>B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="16">
+        <f>B4+C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="16">
+        <f>B5+C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="16">
+        <f>B6+C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="16">
+        <f>B7+C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="16">
+        <f>B8+C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="16">
+        <f>B9+C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="16">
+        <f>B10+C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="16">
+        <f>B11+C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="16">
+        <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="16">
+        <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="16">
+        <f>B14+C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="16">
+        <f>B15+C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="16">
+        <f>B16+C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="16">
+        <f>B17+C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="16">
+        <f>B18+C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="16">
+        <f>B19+C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="16">
+        <f>B20+C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20</f>
         <v>2</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="16">
+        <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="16">
+        <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="16">
+        <f>B23+C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="16">
+        <f>B24+C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="16">
+        <f>B25+C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25</f>
         <v>3</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="16">
+        <f>B26+C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" t="b">
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="16">
+        <f>B27+C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
+    <sortCondition ref="A2:A27"/>
+  </sortState>
+  <conditionalFormatting sqref="P2:P27">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laborator 02.11.2022 - am adaugat imagine pentru pistolul curent, sunet de fundal, sortare de inamici, si putem impusca inamicii doar la pixelii non-transparenti din imagine
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4ADF78-6BD9-40FC-97D8-D8A65E82B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA3CF1-F57C-4C03-8D51-566D7448987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Marta George</t>
+  </si>
+  <si>
+    <t>Luczo Maria</t>
+  </si>
+  <si>
+    <t>Ilea Crina</t>
   </si>
 </sst>
 </file>
@@ -706,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,7 +787,9 @@
         <v>1</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -793,7 +801,7 @@
       <c r="O2" s="11"/>
       <c r="P2" s="16">
         <f>B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -810,7 +818,9 @@
       <c r="E3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -822,7 +832,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="16">
         <f>B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -837,7 +847,9 @@
       <c r="E4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -849,7 +861,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="16">
         <f>B4+C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -864,7 +876,9 @@
       <c r="E5" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -876,7 +890,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="16">
         <f>B5+C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -926,7 +940,9 @@
       <c r="E7" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -938,7 +954,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="16">
         <f>B7+C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -982,7 +998,9 @@
       <c r="E9" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -994,7 +1012,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="16">
         <f>B9+C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1011,7 +1029,9 @@
       <c r="E10" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1023,7 +1043,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="16">
         <f>B10+C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1042,7 +1062,9 @@
       <c r="E11" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -1054,7 +1076,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="16">
         <f>B11+C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1071,7 +1093,9 @@
         <v>1</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1083,24 +1107,20 @@
       <c r="O12" s="12"/>
       <c r="P12" s="16">
         <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1112,12 +1132,12 @@
       <c r="O13" s="12"/>
       <c r="P13" s="16">
         <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="b">
         <v>1</v>
@@ -1128,10 +1148,10 @@
       <c r="D14" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1148,7 +1168,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="b">
         <v>1</v>
@@ -1162,7 +1182,9 @@
       <c r="E15" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1174,12 +1196,12 @@
       <c r="O15" s="12"/>
       <c r="P15" s="16">
         <f>B15+C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" s="5" t="b">
         <v>1</v>
@@ -1193,7 +1215,9 @@
       <c r="E16" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1205,19 +1229,25 @@
       <c r="O16" s="12"/>
       <c r="P16" s="16">
         <f>B16+C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="D17" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1230,19 +1260,19 @@
       <c r="O17" s="12"/>
       <c r="P17" s="16">
         <f>B17+C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1260,14 +1290,14 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1285,17 +1315,15 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1307,20 +1335,22 @@
       <c r="O20" s="12"/>
       <c r="P20" s="16">
         <f>B20+C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1332,18 +1362,20 @@
       <c r="O21" s="12"/>
       <c r="P21" s="16">
         <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1357,20 +1389,22 @@
       <c r="O22" s="12"/>
       <c r="P22" s="16">
         <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1382,12 +1416,12 @@
       <c r="O23" s="12"/>
       <c r="P23" s="16">
         <f>B23+C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="6" t="b">
@@ -1412,18 +1446,14 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C25" s="6"/>
       <c r="D25" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E25" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -1436,23 +1466,19 @@
       <c r="O25" s="12"/>
       <c r="P25" s="16">
         <f>B25+C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>9</v>
+      <c r="A26" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1465,39 +1491,101 @@
       <c r="O26" s="12"/>
       <c r="P26" s="16">
         <f>B26+C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="13"/>
+      <c r="A27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="12"/>
       <c r="P27" s="16">
         <f>B27+C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="16">
+        <f>B28+C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="16">
+        <f>B29+C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
-    <sortCondition ref="A2:A27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
-  <conditionalFormatting sqref="P2:P27">
+  <conditionalFormatting sqref="P2:P29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
commit la mij de laborator
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA3CF1-F57C-4C03-8D51-566D7448987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AF4260-8483-41AB-98CE-A0434EC5DBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Ilea Crina</t>
+  </si>
+  <si>
+    <t>Farcas Vasile</t>
   </si>
 </sst>
 </file>
@@ -712,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +824,9 @@
       <c r="F3" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -832,7 +837,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="16">
         <f>B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -879,7 +884,9 @@
       <c r="F5" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -890,7 +897,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="16">
         <f>B5+C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -910,7 +917,9 @@
         <v>1</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -921,29 +930,21 @@
       <c r="O6" s="12"/>
       <c r="P6" s="16">
         <f>B6+C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -954,12 +955,12 @@
       <c r="O7" s="12"/>
       <c r="P7" s="16">
         <f>B7+C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>1</v>
@@ -967,10 +968,18 @@
       <c r="C8" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -981,26 +990,22 @@
       <c r="O8" s="12"/>
       <c r="P8" s="16">
         <f>B8+C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="C9" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1012,12 +1017,12 @@
       <c r="O9" s="12"/>
       <c r="P9" s="16">
         <f>B9+C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="b">
@@ -1032,7 +1037,9 @@
       <c r="F10" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1043,23 +1050,21 @@
       <c r="O10" s="12"/>
       <c r="P10" s="16">
         <f>B10+C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="10" t="b">
+      <c r="E11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="10" t="b">
@@ -1076,12 +1081,12 @@
       <c r="O11" s="12"/>
       <c r="P11" s="16">
         <f>B11+C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B12" s="5" t="b">
         <v>1</v>
@@ -1092,7 +1097,9 @@
       <c r="D12" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="F12" s="10" t="b">
         <v>1</v>
       </c>
@@ -1107,18 +1114,24 @@
       <c r="O12" s="12"/>
       <c r="P12" s="16">
         <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6" t="b">
+      <c r="F13" s="10" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="6"/>
@@ -1132,24 +1145,18 @@
       <c r="O13" s="12"/>
       <c r="P13" s="16">
         <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="10" t="b">
+      <c r="F14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="6"/>
@@ -1163,12 +1170,12 @@
       <c r="O14" s="12"/>
       <c r="P14" s="16">
         <f>B14+C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="b">
         <v>1</v>
@@ -1179,9 +1186,7 @@
       <c r="D15" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="10" t="b">
         <v>1</v>
       </c>
@@ -1196,12 +1201,12 @@
       <c r="O15" s="12"/>
       <c r="P15" s="16">
         <f>B15+C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="b">
         <v>1</v>
@@ -1234,7 +1239,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" s="5" t="b">
         <v>1</v>
@@ -1248,7 +1253,9 @@
       <c r="E17" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1260,19 +1267,25 @@
       <c r="O17" s="12"/>
       <c r="P17" s="16">
         <f>B17+C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="D18" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1285,19 +1298,19 @@
       <c r="O18" s="12"/>
       <c r="P18" s="16">
         <f>B18+C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1315,15 +1328,15 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="E20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1340,12 +1353,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6" t="b">
@@ -1362,23 +1373,25 @@
       <c r="O21" s="12"/>
       <c r="P21" s="16">
         <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -1389,22 +1402,22 @@
       <c r="O22" s="12"/>
       <c r="P22" s="16">
         <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1421,15 +1434,17 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1441,18 +1456,18 @@
       <c r="O24" s="12"/>
       <c r="P24" s="16">
         <f>B24+C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -1471,13 +1486,13 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -1496,21 +1511,15 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1522,12 +1531,12 @@
       <c r="O27" s="12"/>
       <c r="P27" s="16">
         <f>B27+C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>9</v>
+      <c r="A28" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6" t="b">
@@ -1542,7 +1551,9 @@
       <c r="F28" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
@@ -1553,39 +1564,72 @@
       <c r="O28" s="12"/>
       <c r="P28" s="16">
         <f>B28+C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="13"/>
+      <c r="A29" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="12"/>
       <c r="P29" s="16">
         <f>B29+C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="16">
+        <f>B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P29">
-    <sortCondition ref="A2:A29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P30">
+    <sortCondition ref="A2:A30"/>
   </sortState>
-  <conditionalFormatting sqref="P2:P29">
+  <conditionalFormatting sqref="P2:P30">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
the base REST API project
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38696819-9C87-4054-BF15-16D431D8A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCCF256-4EC6-4C83-AA14-7E5B66A555EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Farcas Vasile</t>
+  </si>
+  <si>
+    <t>Sarb Maria</t>
   </si>
 </sst>
 </file>
@@ -715,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,7 +808,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="11"/>
       <c r="P2" s="16">
-        <f t="shared" ref="P2:P30" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
+        <f>B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
         <v>5</v>
       </c>
     </row>
@@ -829,7 +832,9 @@
       <c r="G3" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -838,8 +843,8 @@
       <c r="N3" s="6"/>
       <c r="O3" s="12"/>
       <c r="P3" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -867,7 +872,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="12"/>
       <c r="P4" s="16">
-        <f t="shared" si="0"/>
+        <f>B4+C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4</f>
         <v>3</v>
       </c>
     </row>
@@ -889,7 +894,9 @@
       <c r="G5" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -898,8 +905,8 @@
       <c r="N5" s="6"/>
       <c r="O5" s="12"/>
       <c r="P5" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>B5+C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5</f>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -922,7 +929,9 @@
       <c r="G6" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -931,8 +940,8 @@
       <c r="N6" s="6"/>
       <c r="O6" s="12"/>
       <c r="P6" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>B6+C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6</f>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -947,7 +956,9 @@
       <c r="G7" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -956,8 +967,8 @@
       <c r="N7" s="6"/>
       <c r="O7" s="12"/>
       <c r="P7" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>B7+C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7</f>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -982,7 +993,9 @@
       <c r="G8" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -991,8 +1004,8 @@
       <c r="N8" s="6"/>
       <c r="O8" s="12"/>
       <c r="P8" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>B8+C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8</f>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1018,7 +1031,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="12"/>
       <c r="P9" s="16">
-        <f t="shared" si="0"/>
+        <f>B9+C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9</f>
         <v>2</v>
       </c>
     </row>
@@ -1042,7 +1055,9 @@
       <c r="G10" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1051,8 +1066,8 @@
       <c r="N10" s="6"/>
       <c r="O10" s="12"/>
       <c r="P10" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>B10+C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10</f>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1082,7 +1097,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="12"/>
       <c r="P11" s="16">
-        <f t="shared" si="0"/>
+        <f>B11+C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11</f>
         <v>4</v>
       </c>
     </row>
@@ -1115,7 +1130,7 @@
       <c r="N12" s="6"/>
       <c r="O12" s="12"/>
       <c r="P12" s="16">
-        <f t="shared" si="0"/>
+        <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
         <v>5</v>
       </c>
     </row>
@@ -1148,7 +1163,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="12"/>
       <c r="P13" s="16">
-        <f t="shared" si="0"/>
+        <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
         <v>5</v>
       </c>
     </row>
@@ -1173,7 +1188,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="12"/>
       <c r="P14" s="16">
-        <f t="shared" si="0"/>
+        <f>B14+C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14</f>
         <v>1</v>
       </c>
     </row>
@@ -1204,7 +1219,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="12"/>
       <c r="P15" s="16">
-        <f t="shared" si="0"/>
+        <f>B15+C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15</f>
         <v>4</v>
       </c>
     </row>
@@ -1237,7 +1252,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="12"/>
       <c r="P16" s="16">
-        <f t="shared" si="0"/>
+        <f>B16+C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16</f>
         <v>5</v>
       </c>
     </row>
@@ -1272,7 +1287,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="12"/>
       <c r="P17" s="16">
-        <f t="shared" si="0"/>
+        <f>B17+C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17</f>
         <v>6</v>
       </c>
     </row>
@@ -1303,7 +1318,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="12"/>
       <c r="P18" s="16">
-        <f t="shared" si="0"/>
+        <f>B18+C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18</f>
         <v>4</v>
       </c>
     </row>
@@ -1328,7 +1343,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="12"/>
       <c r="P19" s="16">
-        <f t="shared" si="0"/>
+        <f>B19+C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19</f>
         <v>1</v>
       </c>
     </row>
@@ -1353,7 +1368,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="12"/>
       <c r="P20" s="16">
-        <f t="shared" si="0"/>
+        <f>B20+C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20</f>
         <v>1</v>
       </c>
     </row>
@@ -1378,7 +1393,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="12"/>
       <c r="P21" s="16">
-        <f t="shared" si="0"/>
+        <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21</f>
         <v>1</v>
       </c>
     </row>
@@ -1398,7 +1413,9 @@
       <c r="G22" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -1407,8 +1424,8 @@
       <c r="N22" s="6"/>
       <c r="O22" s="12"/>
       <c r="P22" s="16">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22</f>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -1434,7 +1451,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="12"/>
       <c r="P23" s="16">
-        <f t="shared" si="0"/>
+        <f>B23+C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23</f>
         <v>2</v>
       </c>
     </row>
@@ -1463,7 +1480,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="12"/>
       <c r="P24" s="16">
-        <f t="shared" si="0"/>
+        <f>B24+C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24</f>
         <v>3</v>
       </c>
     </row>
@@ -1488,7 +1505,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="12"/>
       <c r="P25" s="16">
-        <f t="shared" si="0"/>
+        <f>B25+C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25</f>
         <v>1</v>
       </c>
     </row>
@@ -1513,7 +1530,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="12"/>
       <c r="P26" s="16">
-        <f t="shared" si="0"/>
+        <f>B26+C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26</f>
         <v>1</v>
       </c>
     </row>
@@ -1538,7 +1555,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="12"/>
       <c r="P27" s="16">
-        <f t="shared" si="0"/>
+        <f>B27+C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27</f>
         <v>1</v>
       </c>
     </row>
@@ -1562,7 +1579,9 @@
       <c r="G28" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -1571,8 +1590,8 @@
       <c r="N28" s="6"/>
       <c r="O28" s="12"/>
       <c r="P28" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>B28+C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28</f>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -1604,40 +1623,65 @@
       <c r="N29" s="6"/>
       <c r="O29" s="12"/>
       <c r="P29" s="16">
-        <f t="shared" si="0"/>
+        <f>B29+C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29</f>
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="16">
+        <f>B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="16">
-        <f t="shared" si="0"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="16">
+        <f>B31+C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P30">
-    <sortCondition ref="A2:A30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P31">
+    <sortCondition ref="A2:A31"/>
   </sortState>
-  <conditionalFormatting sqref="P2:P30">
+  <conditionalFormatting sqref="P2:P31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 16.11.2022 - Am creat un start screen si un status bar
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCCF256-4EC6-4C83-AA14-7E5B66A555EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7909CBEA-C239-4BDC-86AB-38C359452188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +799,9 @@
       <c r="G2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -808,8 +810,8 @@
       <c r="N2" s="4"/>
       <c r="O2" s="11"/>
       <c r="P2" s="16">
-        <f>B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
-        <v>5</v>
+        <f t="shared" ref="P2:P31" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -843,7 +845,7 @@
       <c r="N3" s="6"/>
       <c r="O3" s="12"/>
       <c r="P3" s="16">
-        <f>B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -872,7 +874,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="12"/>
       <c r="P4" s="16">
-        <f>B4+C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -905,7 +907,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="12"/>
       <c r="P5" s="16">
-        <f>B5+C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -940,7 +942,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="12"/>
       <c r="P6" s="16">
-        <f>B6+C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -967,7 +969,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="12"/>
       <c r="P7" s="16">
-        <f>B7+C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1004,7 +1006,7 @@
       <c r="N8" s="6"/>
       <c r="O8" s="12"/>
       <c r="P8" s="16">
-        <f>B8+C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1031,7 +1033,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="12"/>
       <c r="P9" s="16">
-        <f>B9+C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1066,7 +1068,7 @@
       <c r="N10" s="6"/>
       <c r="O10" s="12"/>
       <c r="P10" s="16">
-        <f>B10+C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1097,7 +1099,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="12"/>
       <c r="P11" s="16">
-        <f>B11+C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1121,7 +1123,9 @@
         <v>1</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1130,8 +1134,8 @@
       <c r="N12" s="6"/>
       <c r="O12" s="12"/>
       <c r="P12" s="16">
-        <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1154,7 +1158,9 @@
       <c r="G13" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1163,8 +1169,8 @@
       <c r="N13" s="6"/>
       <c r="O13" s="12"/>
       <c r="P13" s="16">
-        <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1188,7 +1194,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="12"/>
       <c r="P14" s="16">
-        <f>B14+C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1219,7 +1225,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="12"/>
       <c r="P15" s="16">
-        <f>B15+C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1243,7 +1249,9 @@
         <v>1</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -1252,8 +1260,8 @@
       <c r="N16" s="6"/>
       <c r="O16" s="12"/>
       <c r="P16" s="16">
-        <f>B16+C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -1278,7 +1286,9 @@
       <c r="G17" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1287,8 +1297,8 @@
       <c r="N17" s="6"/>
       <c r="O17" s="12"/>
       <c r="P17" s="16">
-        <f>B17+C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1318,7 +1328,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="12"/>
       <c r="P18" s="16">
-        <f>B18+C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1343,7 +1353,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="12"/>
       <c r="P19" s="16">
-        <f>B19+C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1368,7 +1378,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="12"/>
       <c r="P20" s="16">
-        <f>B20+C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1393,7 +1403,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="12"/>
       <c r="P21" s="16">
-        <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1424,7 +1434,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="12"/>
       <c r="P22" s="16">
-        <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1451,7 +1461,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="12"/>
       <c r="P23" s="16">
-        <f>B23+C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1480,7 +1490,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="12"/>
       <c r="P24" s="16">
-        <f>B24+C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1505,7 +1515,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="12"/>
       <c r="P25" s="16">
-        <f>B25+C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1530,7 +1540,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="12"/>
       <c r="P26" s="16">
-        <f>B26+C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1555,7 +1565,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="12"/>
       <c r="P27" s="16">
-        <f>B27+C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1590,7 +1600,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="12"/>
       <c r="P28" s="16">
-        <f>B28+C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1614,7 +1624,9 @@
       <c r="G29" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1623,8 +1635,8 @@
       <c r="N29" s="6"/>
       <c r="O29" s="12"/>
       <c r="P29" s="16">
-        <f>B29+C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -1648,7 +1660,7 @@
       <c r="N30" s="6"/>
       <c r="O30" s="12"/>
       <c r="P30" s="16">
-        <f>B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1673,7 +1685,7 @@
       <c r="N31" s="8"/>
       <c r="O31" s="13"/>
       <c r="P31" s="16">
-        <f>B31+C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 29.11.2022 - pagini cu doar HTML si CSS care simuleaza aspectul proiectului final de FE
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742A3494-A056-4E19-9D2F-59F912B20DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B068923-72A8-4357-8D37-A7E9D7C05BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -170,7 +170,7 @@
     <t>Farcas Vasile</t>
   </si>
   <si>
-    <t>Sarb Maria</t>
+    <t>Sirb Maria</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,10 +840,13 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
       <c r="O3" s="10"/>
       <c r="P3" s="14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -943,10 +946,13 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
       <c r="O7" s="10"/>
       <c r="P7" s="14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -977,10 +983,13 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
       <c r="O8" s="10"/>
       <c r="P8" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1025,10 +1034,13 @@
       <c r="I10" t="b">
         <v>1</v>
       </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
       <c r="O10" s="10"/>
       <c r="P10" s="14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1412,10 +1424,13 @@
       <c r="I28" t="b">
         <v>1</v>
       </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
       <c r="O28" s="10"/>
       <c r="P28" s="14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -1461,10 +1476,13 @@
       <c r="I30" t="b">
         <v>1</v>
       </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
       <c r="O30" s="10"/>
       <c r="P30" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Laborator 39.11.2022 - prezenta
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B068923-72A8-4357-8D37-A7E9D7C05BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529C63CA-3FA3-4FC1-910A-32FAE1F3D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -719,7 +719,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,10 +1459,13 @@
       <c r="I29" t="b">
         <v>1</v>
       </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
       <c r="O29" s="10"/>
       <c r="P29" s="14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
"redder screen when taking damage" - merge putin sacadat, dar e un inceput
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529C63CA-3FA3-4FC1-910A-32FAE1F3D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047C64BD-C8CE-45D5-A744-90829B0D1E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -719,7 +719,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,7 +803,9 @@
       <c r="I2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -811,7 +813,7 @@
       <c r="O2" s="9"/>
       <c r="P2" s="14">
         <f t="shared" ref="P2:P31" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1313,10 +1315,13 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
       <c r="O22" s="10"/>
       <c r="P22" s="14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Laborator 06.12.2022 - am creat o aplicatie Angular  in care (deocamdata) afisam paginile web create la laboratorul precedent
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047C64BD-C8CE-45D5-A744-90829B0D1E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650A4CC2-D7BB-4D63-9BCD-801189FDDE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Sirb Maria</t>
+  </si>
+  <si>
+    <t>Schuller Robert</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +391,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,7 +818,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="9"/>
       <c r="P2" s="14">
-        <f t="shared" ref="P2:P31" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
+        <f t="shared" ref="P2:P32" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
         <v>8</v>
       </c>
     </row>
@@ -821,34 +827,40 @@
         <v>32</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
+      <c r="C3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
       <c r="O3" s="10"/>
       <c r="P3" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -856,18 +868,26 @@
         <v>35</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="10"/>
       <c r="P4" s="14">
         <f t="shared" si="0"/>
@@ -879,24 +899,30 @@
         <v>37</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="10"/>
       <c r="P5" s="14">
         <f t="shared" si="0"/>
@@ -910,24 +936,30 @@
       <c r="B6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
+      <c r="C6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="10"/>
       <c r="P6" s="14">
         <f t="shared" si="0"/>
@@ -939,18 +971,26 @@
         <v>44</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="10"/>
       <c r="P7" s="14">
         <f t="shared" si="0"/>
@@ -964,30 +1004,34 @@
       <c r="B8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
+      <c r="C8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="10"/>
       <c r="P8" s="14">
         <f t="shared" si="0"/>
@@ -1001,9 +1045,20 @@
       <c r="B9" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
+      <c r="C9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="10"/>
       <c r="P9" s="14">
         <f t="shared" si="0"/>
@@ -1015,34 +1070,40 @@
         <v>12</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
+      <c r="C10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="10"/>
       <c r="P10" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1050,25 +1111,34 @@
         <v>14</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
+      <c r="C11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="10"/>
       <c r="P11" s="14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1078,24 +1148,30 @@
       <c r="B12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
+      <c r="C12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="10"/>
       <c r="P12" s="14">
         <f t="shared" si="0"/>
@@ -1109,21 +1185,28 @@
       <c r="B13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
+      <c r="C13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="10"/>
       <c r="P13" s="14">
         <f t="shared" si="0"/>
@@ -1135,9 +1218,20 @@
         <v>43</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="10"/>
       <c r="P14" s="14">
         <f t="shared" si="0"/>
@@ -1151,15 +1245,24 @@
       <c r="B15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
+      <c r="C15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="10"/>
       <c r="P15" s="14">
         <f t="shared" si="0"/>
@@ -1173,28 +1276,36 @@
       <c r="B16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
+      <c r="C16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="10"/>
       <c r="P16" s="14">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -1204,27 +1315,32 @@
       <c r="B17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
+      <c r="C17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="10"/>
       <c r="P17" s="14">
         <f t="shared" si="0"/>
@@ -1238,15 +1354,24 @@
       <c r="B18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
+      <c r="C18" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="10"/>
       <c r="P18" s="14">
         <f t="shared" si="0"/>
@@ -1258,9 +1383,20 @@
         <v>36</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14">
         <f t="shared" si="0"/>
@@ -1272,9 +1408,20 @@
         <v>40</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="10"/>
       <c r="P20" s="14">
         <f t="shared" si="0"/>
@@ -1286,13 +1433,26 @@
         <v>42</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="10"/>
       <c r="P21" s="14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -1300,24 +1460,30 @@
         <v>8</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
+      <c r="C22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="10"/>
       <c r="P22" s="14">
         <f t="shared" si="0"/>
@@ -1329,12 +1495,22 @@
         <v>34</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
+      <c r="C23" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
       <c r="O23" s="10"/>
       <c r="P23" s="14">
         <f t="shared" si="0"/>
@@ -1346,15 +1522,24 @@
         <v>41</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="10"/>
       <c r="P24" s="14">
         <f t="shared" si="0"/>
@@ -1366,9 +1551,20 @@
         <v>11</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
+      <c r="C25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="10"/>
       <c r="P25" s="14">
         <f t="shared" si="0"/>
@@ -1380,9 +1576,20 @@
         <v>38</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="10"/>
       <c r="P26" s="14">
         <f t="shared" si="0"/>
@@ -1394,9 +1601,20 @@
         <v>7</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
+      <c r="C27" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
       <c r="O27" s="10"/>
       <c r="P27" s="14">
         <f t="shared" si="0"/>
@@ -1408,34 +1626,40 @@
         <v>31</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="b">
-        <v>1</v>
-      </c>
+      <c r="C28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
       <c r="O28" s="10"/>
       <c r="P28" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -1443,34 +1667,40 @@
         <v>9</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="b">
-        <v>1</v>
-      </c>
+      <c r="C29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
       <c r="O29" s="10"/>
       <c r="P29" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -1478,42 +1708,78 @@
         <v>45</v>
       </c>
       <c r="B30" s="5"/>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" t="b">
-        <v>1</v>
-      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
       <c r="O30" s="10"/>
       <c r="P30" s="14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="11"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="10"/>
       <c r="P31" s="14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="14">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1522,7 +1788,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P31">
     <sortCondition ref="A2:A31"/>
   </sortState>
-  <conditionalFormatting sqref="P2:P31">
+  <conditionalFormatting sqref="P2:P32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Notele si prezenta pt luna ianuarie
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\MetodeAvansateDeProgramare_2022-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B9ADD1-9BA6-43CC-8526-164AFF7B797A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0997171D-A501-4802-81DD-6FC814EC7BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE27C439-FCDA-4A78-B815-62CA1E58451F}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Bexa Denisa</t>
   </si>
@@ -155,9 +144,6 @@
     <t>Petrut Andreea</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Lucaciu Vlad</t>
   </si>
   <si>
@@ -210,6 +196,36 @@
   </si>
   <si>
     <t>Doodle Jump</t>
+  </si>
+  <si>
+    <t>Donut-area</t>
+  </si>
+  <si>
+    <t>Movie management</t>
+  </si>
+  <si>
+    <t>RPG Shooter</t>
+  </si>
+  <si>
+    <t>Lucuta Gabriel</t>
+  </si>
+  <si>
+    <t>ToH &amp; ToDo List</t>
+  </si>
+  <si>
+    <t>Pacman</t>
+  </si>
+  <si>
+    <t>Prezente</t>
+  </si>
+  <si>
+    <t>RPG</t>
+  </si>
+  <si>
+    <t>Personal Website</t>
+  </si>
+  <si>
+    <t>Car Racing</t>
   </si>
 </sst>
 </file>
@@ -259,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -389,10 +405,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -405,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,10 +462,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -750,7 +797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -758,16 +805,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DE6A8-48D8-4F4C-AA06-F014A798D754}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="17" max="17" width="17.88671875" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -817,13 +865,13 @@
         <v>30</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -858,16 +906,23 @@
       <c r="K2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="14">
-        <f t="shared" ref="P2:P32" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
-        <v>9</v>
+      <c r="O2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="18">
+        <f t="shared" ref="P2:P33" si="0">B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2</f>
+        <v>11</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="R2" s="15">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -905,12 +960,25 @@
       <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="14">
-        <f t="shared" si="0"/>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" s="18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="14">
         <v>10</v>
       </c>
-      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -932,13 +1000,18 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>51</v>
+      <c r="O4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="14">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -967,13 +1040,24 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="14">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>52</v>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="14">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1004,16 +1088,26 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="14">
-        <f t="shared" si="0"/>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="R6" s="14">
         <v>8</v>
       </c>
-      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5"/>
       <c r="G7" t="b">
@@ -1028,12 +1122,22 @@
       <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q7" s="15"/>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -1066,12 +1170,25 @@
       <c r="J8" t="b">
         <v>1</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="14">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="Q8" s="15"/>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -1084,11 +1201,14 @@
         <v>1</v>
       </c>
       <c r="O9" s="10"/>
-      <c r="P9" s="14">
+      <c r="P9" s="18">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
@@ -1125,13 +1245,24 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="14">
-        <f t="shared" si="0"/>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10" s="14">
         <v>10</v>
-      </c>
-      <c r="Q10" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1160,12 +1291,17 @@
       <c r="L11" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="14">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Q11" s="15"/>
+      <c r="O11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" s="18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
@@ -1195,12 +1331,20 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
       <c r="O12" s="10"/>
-      <c r="P12" s="14">
-        <f>B12+C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12</f>
-        <v>8</v>
-      </c>
-      <c r="Q12" s="15"/>
+      <c r="P12" s="18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R12" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
@@ -1225,26 +1369,36 @@
         <v>1</v>
       </c>
       <c r="O13" s="10"/>
-      <c r="P13" s="14">
-        <f>B13+C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13</f>
+      <c r="P13" s="18">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q13" s="15"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5"/>
       <c r="F14" t="b">
         <v>1</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="15"/>
+      <c r="O14" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
@@ -1265,12 +1419,19 @@
       <c r="L15" t="b">
         <v>1</v>
       </c>
-      <c r="O15" s="10"/>
-      <c r="P15" s="14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q15" s="15"/>
+      <c r="O15" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R15" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
@@ -1300,12 +1461,19 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="14">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q16" s="15"/>
+      <c r="O16" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" s="18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R16" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
@@ -1338,13 +1506,24 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="O17" s="10"/>
-      <c r="P17" s="14">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="Q17" s="15" t="s">
-        <v>54</v>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="R17" s="14">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -1364,11 +1543,14 @@
         <v>1</v>
       </c>
       <c r="O18" s="10"/>
-      <c r="P18" s="14">
+      <c r="P18" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Q18" s="15"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
@@ -1379,219 +1561,224 @@
         <v>1</v>
       </c>
       <c r="O19" s="10"/>
-      <c r="P19" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q19" s="15"/>
+      <c r="P19" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5"/>
       <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="O20" s="10"/>
-      <c r="P20" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q20" s="15"/>
+      <c r="P20" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="10"/>
-      <c r="P21" s="14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q21" s="15"/>
+      <c r="O21" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R21" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
       <c r="K22" t="b">
         <v>1</v>
       </c>
       <c r="O22" s="10"/>
-      <c r="P22" s="14">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Q22" s="15" t="s">
-        <v>55</v>
+      <c r="P22" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" t="b">
         <v>1</v>
       </c>
-      <c r="D23" t="b">
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="b">
         <v>1</v>
       </c>
       <c r="O23" s="10"/>
-      <c r="P23" s="14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q23" s="15"/>
+      <c r="P23" s="18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="R23" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="O24" s="10"/>
-      <c r="P24" s="14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q24" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="R24" s="15">
-        <v>10</v>
+      <c r="P24" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" t="b">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
         <v>1</v>
       </c>
       <c r="O25" s="10"/>
-      <c r="P25" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q25" s="15"/>
+      <c r="P25" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="R25" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="D26" t="b">
+      <c r="C26" t="b">
         <v>1</v>
       </c>
       <c r="O26" s="10"/>
-      <c r="P26" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q26" s="15"/>
+      <c r="P26" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" t="b">
+      <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="O27" s="10"/>
-      <c r="P27" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q27" s="15"/>
+      <c r="P27" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" t="b">
         <v>1</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="b">
-        <v>1</v>
-      </c>
-      <c r="L28" t="b">
-        <v>1</v>
-      </c>
       <c r="O28" s="10"/>
-      <c r="P28" s="14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="Q28" s="15" t="s">
-        <v>56</v>
+      <c r="P28" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" t="b">
@@ -1624,20 +1811,46 @@
       <c r="L29" t="b">
         <v>1</v>
       </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="14">
-        <f t="shared" si="0"/>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" s="14">
         <v>10</v>
-      </c>
-      <c r="Q29" s="15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B30" s="5"/>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
       <c r="H30" t="b">
         <v>1</v>
       </c>
@@ -1653,59 +1866,111 @@
       <c r="L30" t="b">
         <v>1</v>
       </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" t="b">
+        <v>1</v>
+      </c>
       <c r="O30" s="10"/>
-      <c r="P30" s="14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q30" s="15"/>
+      <c r="P30" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="R30" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" t="b">
+      <c r="K31" t="b">
         <v>1</v>
       </c>
       <c r="O31" s="10"/>
-      <c r="P31" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q31" s="15"/>
+      <c r="P31" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q32" s="15"/>
+        <v>44</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="10"/>
+      <c r="P32" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q32" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="R32" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P31">
-    <sortCondition ref="A2:A31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
-  <conditionalFormatting sqref="P2:P32">
+  <conditionalFormatting sqref="P2:P33">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>